<commit_message>
modefied mibirem standardization template and raw data for T 0,1,2 and 3
</commit_message>
<xml_diff>
--- a/data/mibirem_standard_data_templates/TemplateData_W.xlsx
+++ b/data/mibirem_standard_data_templates/TemplateData_W.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseye001\Sona_Phd\MIBIREM\MiBiPreT_FieldSites\constructed-wetland\data\mibirem_standard_data_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A20769-8575-4DDE-ABE7-E164518A7E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB42DC17-FD37-41BB-8305-B32345267B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chemical analysis" sheetId="1" r:id="rId1"/>
@@ -440,136 +440,136 @@
     <t>total oil C10 - C40</t>
   </si>
   <si>
-    <t>INF(INF-1-4)</t>
-  </si>
-  <si>
     <t>INF</t>
   </si>
   <si>
-    <t>CW1_EFF(CW1_EFF-1-4)</t>
-  </si>
-  <si>
     <t>CW1_EFF</t>
   </si>
   <si>
-    <t>CW1MF01(CW1MF01-1-5)</t>
-  </si>
-  <si>
     <t>CW1MF01</t>
   </si>
   <si>
-    <t>CW1MF02(CW1MF02-1-5)</t>
-  </si>
-  <si>
     <t>CW1MF02</t>
   </si>
   <si>
-    <t>CW1MF05(CW1MF05-1-4)</t>
-  </si>
-  <si>
     <t>CW1MF05</t>
   </si>
   <si>
-    <t>CW1MF06(CW1MF06-1-4)</t>
-  </si>
-  <si>
     <t>CW1MF06</t>
   </si>
   <si>
-    <t>CW1MF09(CW1MF09-1-5)</t>
-  </si>
-  <si>
     <t>CW1MF09</t>
   </si>
   <si>
-    <t>CW1MF10(CW1MF10-1-5)</t>
-  </si>
-  <si>
     <t>CW1MF10</t>
   </si>
   <si>
-    <t>CW2_EFF(CW2_EFF-1-5)</t>
-  </si>
-  <si>
     <t>CW2_EFF</t>
   </si>
   <si>
-    <t>CW2MF01(CW2MF01-1-4)</t>
-  </si>
-  <si>
     <t>CW2MF01</t>
   </si>
   <si>
-    <t>CW2MF02(CW2MF02-1-4)</t>
-  </si>
-  <si>
     <t>CW2MF02</t>
   </si>
   <si>
-    <t>CW2MF05(CW2MF05-1-4)</t>
-  </si>
-  <si>
     <t>CW2MF05</t>
   </si>
   <si>
-    <t>CW2MF06(CW2MF06-1-4)</t>
-  </si>
-  <si>
     <t>CW2MF06</t>
   </si>
   <si>
-    <t>CW2MF09(CW2MF09-1-4)</t>
-  </si>
-  <si>
     <t>CW2MF09</t>
   </si>
   <si>
-    <t>CW2MF10(CW2MF10-1-4)</t>
-  </si>
-  <si>
     <t>CW2MF10</t>
   </si>
   <si>
-    <t>CW3_EFF(CW3_EFF-1-4)</t>
-  </si>
-  <si>
     <t>CW3_EFF</t>
   </si>
   <si>
-    <t>CW3MF01(CW3MF01-1-4)</t>
-  </si>
-  <si>
     <t>CW3MF01</t>
   </si>
   <si>
-    <t>CW3MF02(CW3MF02-1-4)</t>
-  </si>
-  <si>
     <t>CW3MF02</t>
   </si>
   <si>
-    <t>CW3MF05(CW3MF05-1-4)</t>
-  </si>
-  <si>
     <t>CW3MF05</t>
   </si>
   <si>
-    <t>CW3MF06(CW3MF06-1-4)</t>
-  </si>
-  <si>
     <t>CW3MF06</t>
   </si>
   <si>
-    <t>CW3MF09(CW3MF09-1-4)</t>
-  </si>
-  <si>
     <t>CW3MF09</t>
   </si>
   <si>
-    <t>CW3MF10(CW3MF10-1-4)</t>
-  </si>
-  <si>
     <t>CW3MF10</t>
+  </si>
+  <si>
+    <t>CW1MF05-1-4</t>
+  </si>
+  <si>
+    <t>CW1MF02-1-5</t>
+  </si>
+  <si>
+    <t>CW1MF01-1-5</t>
+  </si>
+  <si>
+    <t>CW1MF06-1-4</t>
+  </si>
+  <si>
+    <t>CW1MF09-1-5</t>
+  </si>
+  <si>
+    <t>CW1MF10-1-5</t>
+  </si>
+  <si>
+    <t>CW1_EFF-1-4</t>
+  </si>
+  <si>
+    <t>CW2MF01-1-4</t>
+  </si>
+  <si>
+    <t>CW2MF02-1-4</t>
+  </si>
+  <si>
+    <t>CW2MF05-1-4</t>
+  </si>
+  <si>
+    <t>CW2MF06-1-4</t>
+  </si>
+  <si>
+    <t>CW2MF09-1-4</t>
+  </si>
+  <si>
+    <t>CW2MF10-1-4</t>
+  </si>
+  <si>
+    <t>CW2_EFF-1-5</t>
+  </si>
+  <si>
+    <t>CW3MF01-1-4</t>
+  </si>
+  <si>
+    <t>CW3MF02-1-4</t>
+  </si>
+  <si>
+    <t>CW3MF05-1-4</t>
+  </si>
+  <si>
+    <t>CW3MF06-1-4</t>
+  </si>
+  <si>
+    <t>CW3MF09-1-4</t>
+  </si>
+  <si>
+    <t>CW3MF10-1-4</t>
+  </si>
+  <si>
+    <t>CW3_EFF-1-4</t>
+  </si>
+  <si>
+    <t>INF-1-4</t>
   </si>
 </sst>
 </file>
@@ -885,8 +885,8 @@
   </sheetPr>
   <dimension ref="A1:DM24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -898,7 +898,7 @@
     <col min="54" max="54" width="21.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:117" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:117" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:117" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:117" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>104</v>
       </c>
@@ -1604,12 +1604,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:117" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:117" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>139</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>140</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1639,12 +1639,12 @@
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
     </row>
-    <row r="4" spans="1:117" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:117" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>142</v>
       </c>
       <c r="BX4" s="1"/>
       <c r="BY4" s="1"/>
@@ -1654,12 +1654,12 @@
       <c r="CC4" s="1"/>
       <c r="CD4" s="1"/>
     </row>
-    <row r="5" spans="1:117" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:117" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="BX5" s="1"/>
       <c r="BY5" s="1"/>
@@ -1671,146 +1671,146 @@
     </row>
     <row r="6" spans="1:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1818,7 +1818,7 @@
         <v>181</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1833,8 +1833,8 @@
   </sheetPr>
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1842,7 +1842,7 @@
     <col min="3" max="3" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>104</v>
       </c>
@@ -1946,172 +1946,172 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>139</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2119,7 +2119,7 @@
         <v>181</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>